<commit_message>
Finished cleaning of data for sheet 8
</commit_message>
<xml_diff>
--- a/webscraper/templates/TemplateA&L.xlsx
+++ b/webscraper/templates/TemplateA&L.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32696" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32704" uniqueCount="161">
   <si>
     <t>FYear</t>
   </si>
@@ -854,7 +854,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4087"/>
+  <dimension ref="A1:H4088"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -107122,6 +107122,32 @@
         <v>159</v>
       </c>
     </row>
+    <row r="4088" spans="1:8">
+      <c r="A4088" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4088" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4088" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4088" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4088" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4088" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4088" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4088" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>